<commit_message>
hien popup huy nhan thung
</commit_message>
<xml_diff>
--- a/Data_Product/App_Data/QTGN_Gang_Long_PKH.xlsx
+++ b/Data_Product/App_Data/QTGN_Gang_Long_PKH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Projects\DATAPRODUCT\DATAPRODUCT\Data_Product\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D53039-5D5C-41FA-AE7A-81E996398434}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09A357A-F50D-469D-BE37-14397545722F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12105" xr2:uid="{51577134-7CEF-4490-9A02-725D1462A1F6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>STT</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>Chuyển đến</t>
+  </si>
+  <si>
+    <t>KL gang nhận (T)</t>
+  </si>
+  <si>
+    <t>KL phế (T)</t>
   </si>
 </sst>
 </file>
@@ -336,6 +342,12 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -347,12 +359,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -712,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC901D94-D8FD-44B6-9D08-9B52821867A9}">
-  <dimension ref="A1:AE11"/>
+  <dimension ref="A1:AG11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="Y4" workbookViewId="0">
+      <selection activeCell="AI13" sqref="AI13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,146 +747,151 @@
     <col min="19" max="19" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="33.28515625" style="2" customWidth="1"/>
-    <col min="22" max="22" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="26" width="9.140625" style="2"/>
-    <col min="27" max="27" width="19.28515625" style="2" customWidth="1"/>
-    <col min="28" max="28" width="19.5703125" style="2" customWidth="1"/>
-    <col min="29" max="29" width="9.140625" style="2"/>
-    <col min="30" max="30" width="25.5703125" style="2" customWidth="1"/>
-    <col min="31" max="31" width="17.140625" style="2" customWidth="1"/>
-    <col min="32" max="16384" width="9.140625" style="2"/>
+    <col min="22" max="22" width="14.85546875" style="2" customWidth="1"/>
+    <col min="23" max="23" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="28" width="9.140625" style="2"/>
+    <col min="29" max="29" width="19.28515625" style="2" customWidth="1"/>
+    <col min="30" max="30" width="19.5703125" style="2" customWidth="1"/>
+    <col min="31" max="31" width="9.140625" style="2"/>
+    <col min="32" max="32" width="25.5703125" style="2" customWidth="1"/>
+    <col min="33" max="33" width="17.140625" style="2" customWidth="1"/>
+    <col min="34" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+    <row r="1" spans="1:33" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
     </row>
-    <row r="2" spans="1:31" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
+    <row r="2" spans="1:33" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
     </row>
-    <row r="4" spans="1:31" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:33" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="20"/>
-      <c r="U4" s="20"/>
-      <c r="V4" s="20"/>
-      <c r="W4" s="20"/>
-      <c r="X4" s="20"/>
-      <c r="Y4" s="20"/>
-      <c r="Z4" s="20"/>
-      <c r="AA4" s="20"/>
-      <c r="AB4" s="20"/>
-      <c r="AC4" s="20"/>
-      <c r="AD4" s="20"/>
-      <c r="AE4" s="20"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="22"/>
+      <c r="Y4" s="22"/>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="22"/>
+      <c r="AB4" s="22"/>
+      <c r="AC4" s="22"/>
+      <c r="AD4" s="22"/>
+      <c r="AE4" s="22"/>
+      <c r="AF4" s="22"/>
+      <c r="AG4" s="22"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="17"/>
-      <c r="U5" s="17"/>
-      <c r="V5" s="17"/>
-      <c r="W5" s="17"/>
-      <c r="X5" s="17"/>
-      <c r="Y5" s="17"/>
-      <c r="Z5" s="17"/>
-      <c r="AA5" s="17"/>
-      <c r="AB5" s="17"/>
-      <c r="AC5" s="17"/>
-      <c r="AD5" s="17"/>
-      <c r="AE5" s="17"/>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="19"/>
+      <c r="W5" s="19"/>
+      <c r="X5" s="19"/>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="19"/>
+      <c r="AA5" s="19"/>
+      <c r="AB5" s="19"/>
+      <c r="AC5" s="19"/>
+      <c r="AD5" s="19"/>
+      <c r="AE5" s="19"/>
+      <c r="AF5" s="19"/>
+      <c r="AG5" s="19"/>
     </row>
-    <row r="7" spans="1:31" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+    <row r="7" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="22" t="s">
+      <c r="J7" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="21" t="s">
+      <c r="K7" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="L7" s="21" t="s">
+      <c r="L7" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="M7" s="21" t="s">
+      <c r="M7" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="N7" s="21" t="s">
+      <c r="N7" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="O7" s="21" t="s">
+      <c r="O7" s="17" t="s">
         <v>31</v>
       </c>
       <c r="P7" s="16" t="s">
@@ -902,37 +913,43 @@
         <v>1</v>
       </c>
       <c r="V7" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="W7" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="W7" s="13" t="s">
+      <c r="X7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="X7" s="13" t="s">
+      <c r="Y7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="Y7" s="13" t="s">
+      <c r="Z7" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="Z7" s="13" t="s">
+      <c r="AA7" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="AA7" s="13" t="s">
+      <c r="AC7" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="AB7" s="15" t="s">
+      <c r="AD7" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AC7" s="14" t="s">
+      <c r="AE7" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="AD7" s="14" t="s">
+      <c r="AF7" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="AE7" s="14" t="s">
+      <c r="AG7" s="14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -960,12 +977,14 @@
       <c r="Y8" s="9"/>
       <c r="Z8" s="9"/>
       <c r="AA8" s="9"/>
-      <c r="AB8" s="11"/>
-      <c r="AC8" s="11"/>
+      <c r="AB8" s="9"/>
+      <c r="AC8" s="9"/>
       <c r="AD8" s="11"/>
       <c r="AE8" s="11"/>
+      <c r="AF8" s="11"/>
+      <c r="AG8" s="11"/>
     </row>
-    <row r="9" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -981,9 +1000,9 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="7"/>
-      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
     </row>
-    <row r="10" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -999,9 +1018,9 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="7"/>
-      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
     </row>
-    <row r="11" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -1017,13 +1036,13 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="7"/>
-      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A5:AE5"/>
+    <mergeCell ref="A5:AG5"/>
     <mergeCell ref="B1:H2"/>
-    <mergeCell ref="A4:AE4"/>
+    <mergeCell ref="A4:AG4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
sua export excel pkh
</commit_message>
<xml_diff>
--- a/Data_Product/App_Data/QTGN_Gang_Long_PKH.xlsx
+++ b/Data_Product/App_Data/QTGN_Gang_Long_PKH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Projects\DATAPRODUCT\DATAPRODUCT\Data_Product\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09A357A-F50D-469D-BE37-14397545722F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC5A155-994D-4767-97B5-A10F400DF6DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12105" xr2:uid="{51577134-7CEF-4490-9A02-725D1462A1F6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>STT</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>KL phế (T)</t>
+  </si>
+  <si>
+    <t>KL gang lỏng (T)</t>
   </si>
 </sst>
 </file>
@@ -718,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC901D94-D8FD-44B6-9D08-9B52821867A9}">
-  <dimension ref="A1:AG11"/>
+  <dimension ref="A1:AJ11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y4" workbookViewId="0">
-      <selection activeCell="AI13" sqref="AI13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,7 +739,7 @@
     <col min="8" max="8" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.42578125" style="1" customWidth="1"/>
     <col min="10" max="10" width="12.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" style="1" customWidth="1"/>
     <col min="12" max="12" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -747,18 +750,23 @@
     <col min="19" max="19" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="33.28515625" style="2" customWidth="1"/>
-    <col min="22" max="22" width="14.85546875" style="2" customWidth="1"/>
-    <col min="23" max="23" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="28" width="9.140625" style="2"/>
-    <col min="29" max="29" width="19.28515625" style="2" customWidth="1"/>
-    <col min="30" max="30" width="19.5703125" style="2" customWidth="1"/>
-    <col min="31" max="31" width="9.140625" style="2"/>
-    <col min="32" max="32" width="25.5703125" style="2" customWidth="1"/>
-    <col min="33" max="33" width="17.140625" style="2" customWidth="1"/>
-    <col min="34" max="16384" width="9.140625" style="2"/>
+    <col min="22" max="22" width="12" style="2" customWidth="1"/>
+    <col min="23" max="23" width="9.7109375" style="2" customWidth="1"/>
+    <col min="24" max="24" width="9.42578125" style="2" customWidth="1"/>
+    <col min="25" max="25" width="10.42578125" style="2" customWidth="1"/>
+    <col min="26" max="26" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.140625" style="2"/>
+    <col min="28" max="29" width="10.7109375" style="2" customWidth="1"/>
+    <col min="30" max="31" width="10.85546875" style="2" customWidth="1"/>
+    <col min="32" max="32" width="19.28515625" style="2" customWidth="1"/>
+    <col min="33" max="33" width="19.5703125" style="2" customWidth="1"/>
+    <col min="34" max="34" width="9.140625" style="2"/>
+    <col min="35" max="35" width="25.5703125" style="2" customWidth="1"/>
+    <col min="36" max="36" width="17.140625" style="2" customWidth="1"/>
+    <col min="37" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
       <c r="D1" s="20"/>
@@ -767,7 +775,7 @@
       <c r="G1" s="21"/>
       <c r="H1" s="21"/>
     </row>
-    <row r="2" spans="1:33" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
@@ -776,7 +784,7 @@
       <c r="G2" s="21"/>
       <c r="H2" s="21"/>
     </row>
-    <row r="4" spans="1:33" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>8</v>
       </c>
@@ -812,8 +820,11 @@
       <c r="AE4" s="22"/>
       <c r="AF4" s="22"/>
       <c r="AG4" s="22"/>
+      <c r="AH4" s="22"/>
+      <c r="AI4" s="22"/>
+      <c r="AJ4" s="22"/>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="19"/>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
@@ -847,8 +858,11 @@
       <c r="AE5" s="19"/>
       <c r="AF5" s="19"/>
       <c r="AG5" s="19"/>
+      <c r="AH5" s="19"/>
+      <c r="AI5" s="19"/>
+      <c r="AJ5" s="19"/>
     </row>
-    <row r="7" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>0</v>
       </c>
@@ -913,43 +927,52 @@
         <v>1</v>
       </c>
       <c r="V7" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="W7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="X7" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y7" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="W7" s="13" t="s">
+      <c r="Z7" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="X7" s="13" t="s">
+      <c r="AA7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="Y7" s="13" t="s">
+      <c r="AB7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="Z7" s="13" t="s">
+      <c r="AC7" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="AA7" s="13" t="s">
+      <c r="AD7" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="AB7" s="13" t="s">
+      <c r="AE7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="AC7" s="13" t="s">
+      <c r="AF7" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="AD7" s="15" t="s">
+      <c r="AG7" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AE7" s="14" t="s">
+      <c r="AH7" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="AF7" s="14" t="s">
+      <c r="AI7" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="AG7" s="14" t="s">
+      <c r="AJ7" s="14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -979,12 +1002,15 @@
       <c r="AA8" s="9"/>
       <c r="AB8" s="9"/>
       <c r="AC8" s="9"/>
-      <c r="AD8" s="11"/>
-      <c r="AE8" s="11"/>
-      <c r="AF8" s="11"/>
+      <c r="AD8" s="9"/>
+      <c r="AE8" s="9"/>
+      <c r="AF8" s="9"/>
       <c r="AG8" s="11"/>
+      <c r="AH8" s="11"/>
+      <c r="AI8" s="11"/>
+      <c r="AJ8" s="11"/>
     </row>
-    <row r="9" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -1000,9 +1026,9 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="7"/>
-      <c r="W9" s="3"/>
+      <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1018,9 +1044,9 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="7"/>
-      <c r="W10" s="3"/>
+      <c r="Z10" s="3"/>
     </row>
-    <row r="11" spans="1:33" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -1036,13 +1062,13 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="7"/>
-      <c r="W11" s="3"/>
+      <c r="Z11" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A5:AG5"/>
+    <mergeCell ref="A5:AJ5"/>
     <mergeCell ref="B1:H2"/>
-    <mergeCell ref="A4:AG4"/>
+    <mergeCell ref="A4:AJ4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
them 2 column moi cho phan ke hoach
</commit_message>
<xml_diff>
--- a/Data_Product/App_Data/QTGN_Gang_Long_PKH.xlsx
+++ b/Data_Product/App_Data/QTGN_Gang_Long_PKH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Projects\DATAPRODUCT\DATAPRODUCT\Data_Product\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC5A155-994D-4767-97B5-A10F400DF6DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E823D389-BEE9-4EFA-844B-E8B8D7FE70FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12105" xr2:uid="{51577134-7CEF-4490-9A02-725D1462A1F6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>STT</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>KL gang lỏng (T)</t>
+  </si>
+  <si>
+    <t>Giờ bắt đầu thổi</t>
   </si>
 </sst>
 </file>
@@ -721,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC901D94-D8FD-44B6-9D08-9B52821867A9}">
-  <dimension ref="A1:AJ11"/>
+  <dimension ref="A1:AK11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="Q4" workbookViewId="0">
+      <selection activeCell="AG10" sqref="AG10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,15 +761,15 @@
     <col min="27" max="27" width="9.140625" style="2"/>
     <col min="28" max="29" width="10.7109375" style="2" customWidth="1"/>
     <col min="30" max="31" width="10.85546875" style="2" customWidth="1"/>
-    <col min="32" max="32" width="19.28515625" style="2" customWidth="1"/>
-    <col min="33" max="33" width="19.5703125" style="2" customWidth="1"/>
-    <col min="34" max="34" width="9.140625" style="2"/>
-    <col min="35" max="35" width="25.5703125" style="2" customWidth="1"/>
-    <col min="36" max="36" width="17.140625" style="2" customWidth="1"/>
-    <col min="37" max="16384" width="9.140625" style="2"/>
+    <col min="32" max="33" width="19.28515625" style="2" customWidth="1"/>
+    <col min="34" max="34" width="19.5703125" style="2" customWidth="1"/>
+    <col min="35" max="35" width="9.140625" style="2"/>
+    <col min="36" max="36" width="25.5703125" style="2" customWidth="1"/>
+    <col min="37" max="37" width="17.140625" style="2" customWidth="1"/>
+    <col min="38" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
       <c r="D1" s="20"/>
@@ -775,7 +778,7 @@
       <c r="G1" s="21"/>
       <c r="H1" s="21"/>
     </row>
-    <row r="2" spans="1:36" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
@@ -784,7 +787,7 @@
       <c r="G2" s="21"/>
       <c r="H2" s="21"/>
     </row>
-    <row r="4" spans="1:36" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:37" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>8</v>
       </c>
@@ -823,8 +826,9 @@
       <c r="AH4" s="22"/>
       <c r="AI4" s="22"/>
       <c r="AJ4" s="22"/>
+      <c r="AK4" s="22"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="19"/>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
@@ -861,8 +865,9 @@
       <c r="AH5" s="19"/>
       <c r="AI5" s="19"/>
       <c r="AJ5" s="19"/>
+      <c r="AK5" s="19"/>
     </row>
-    <row r="7" spans="1:36" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>0</v>
       </c>
@@ -959,20 +964,23 @@
       <c r="AF7" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="AG7" s="15" t="s">
+      <c r="AG7" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH7" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AH7" s="14" t="s">
+      <c r="AI7" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="AI7" s="14" t="s">
+      <c r="AJ7" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="AJ7" s="14" t="s">
+      <c r="AK7" s="14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -1005,12 +1013,13 @@
       <c r="AD8" s="9"/>
       <c r="AE8" s="9"/>
       <c r="AF8" s="9"/>
-      <c r="AG8" s="11"/>
+      <c r="AG8" s="9"/>
       <c r="AH8" s="11"/>
       <c r="AI8" s="11"/>
       <c r="AJ8" s="11"/>
+      <c r="AK8" s="11"/>
     </row>
-    <row r="9" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:37" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -1028,7 +1037,7 @@
       <c r="P9" s="7"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:37" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1046,7 +1055,7 @@
       <c r="P10" s="7"/>
       <c r="Z10" s="3"/>
     </row>
-    <row r="11" spans="1:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:37" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -1066,9 +1075,9 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A5:AJ5"/>
+    <mergeCell ref="A5:AK5"/>
     <mergeCell ref="B1:H2"/>
-    <mergeCell ref="A4:AJ4"/>
+    <mergeCell ref="A4:AK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix bug theo yeu cau NM
</commit_message>
<xml_diff>
--- a/Data_Product/App_Data/QTGN_Gang_Long_PKH.xlsx
+++ b/Data_Product/App_Data/QTGN_Gang_Long_PKH.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Projects\DATAPRODUCT\DATAPRODUCT\Data_Product\App_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_Projects\DATAPRODUCT\DATAPRODUCT\Data_Product\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E823D389-BEE9-4EFA-844B-E8B8D7FE70FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4DF576-4B5D-4BA5-87ED-2D2381A7ACC2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12105" xr2:uid="{51577134-7CEF-4490-9A02-725D1462A1F6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="36">
   <si>
     <t>STT</t>
   </si>
@@ -139,7 +139,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,56 +169,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="13"/>
-      <color theme="1" tint="4.9989318521683403E-2"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color theme="1" tint="4.9989318521683403E-2"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="1" tint="4.9989318521683403E-2"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <name val="Arial"/>
@@ -244,6 +194,35 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -308,50 +287,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -365,6 +321,30 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -724,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC901D94-D8FD-44B6-9D08-9B52821867A9}">
-  <dimension ref="A1:AK11"/>
+  <dimension ref="A1:AR29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q4" workbookViewId="0">
-      <selection activeCell="AG10" sqref="AG10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,12 +719,12 @@
     <col min="5" max="5" width="24.140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.42578125" style="1" customWidth="1"/>
     <col min="10" max="10" width="12.42578125" style="1" customWidth="1"/>
     <col min="11" max="11" width="9.42578125" style="1" customWidth="1"/>
     <col min="12" max="12" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.85546875" style="2" customWidth="1"/>
     <col min="16" max="16" width="10.42578125" style="2" customWidth="1"/>
@@ -769,309 +749,1228 @@
     <col min="38" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-    </row>
-    <row r="2" spans="1:37" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-    </row>
-    <row r="4" spans="1:37" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
+    <row r="1" spans="1:44" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+    </row>
+    <row r="2" spans="1:44" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+    </row>
+    <row r="4" spans="1:44" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
-      <c r="S4" s="22"/>
-      <c r="T4" s="22"/>
-      <c r="U4" s="22"/>
-      <c r="V4" s="22"/>
-      <c r="W4" s="22"/>
-      <c r="X4" s="22"/>
-      <c r="Y4" s="22"/>
-      <c r="Z4" s="22"/>
-      <c r="AA4" s="22"/>
-      <c r="AB4" s="22"/>
-      <c r="AC4" s="22"/>
-      <c r="AD4" s="22"/>
-      <c r="AE4" s="22"/>
-      <c r="AF4" s="22"/>
-      <c r="AG4" s="22"/>
-      <c r="AH4" s="22"/>
-      <c r="AI4" s="22"/>
-      <c r="AJ4" s="22"/>
-      <c r="AK4" s="22"/>
-    </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="19"/>
-      <c r="S5" s="19"/>
-      <c r="T5" s="19"/>
-      <c r="U5" s="19"/>
-      <c r="V5" s="19"/>
-      <c r="W5" s="19"/>
-      <c r="X5" s="19"/>
-      <c r="Y5" s="19"/>
-      <c r="Z5" s="19"/>
-      <c r="AA5" s="19"/>
-      <c r="AB5" s="19"/>
-      <c r="AC5" s="19"/>
-      <c r="AD5" s="19"/>
-      <c r="AE5" s="19"/>
-      <c r="AF5" s="19"/>
-      <c r="AG5" s="19"/>
-      <c r="AH5" s="19"/>
-      <c r="AI5" s="19"/>
-      <c r="AJ5" s="19"/>
-      <c r="AK5" s="19"/>
-    </row>
-    <row r="7" spans="1:37" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="13"/>
+      <c r="U4" s="13"/>
+      <c r="V4" s="13"/>
+      <c r="W4" s="13"/>
+      <c r="X4" s="13"/>
+      <c r="Y4" s="13"/>
+      <c r="Z4" s="13"/>
+      <c r="AA4" s="13"/>
+      <c r="AB4" s="13"/>
+      <c r="AC4" s="13"/>
+      <c r="AD4" s="13"/>
+      <c r="AE4" s="13"/>
+      <c r="AF4" s="13"/>
+      <c r="AG4" s="13"/>
+      <c r="AH4" s="13"/>
+      <c r="AI4" s="13"/>
+      <c r="AJ4" s="13"/>
+      <c r="AK4" s="13"/>
+    </row>
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="10"/>
+      <c r="AA5" s="10"/>
+      <c r="AB5" s="10"/>
+      <c r="AC5" s="10"/>
+      <c r="AD5" s="10"/>
+      <c r="AE5" s="10"/>
+      <c r="AF5" s="10"/>
+      <c r="AG5" s="10"/>
+      <c r="AH5" s="10"/>
+      <c r="AI5" s="10"/>
+      <c r="AJ5" s="10"/>
+      <c r="AK5" s="10"/>
+    </row>
+    <row r="7" spans="1:44" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="18" t="s">
+      <c r="J7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="L7" s="17" t="s">
+      <c r="L7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="M7" s="17" t="s">
+      <c r="M7" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="N7" s="17" t="s">
+      <c r="N7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="O7" s="17" t="s">
+      <c r="O7" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="P7" s="16" t="s">
+      <c r="P7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="Q7" s="16" t="s">
+      <c r="Q7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="R7" s="13" t="s">
+      <c r="R7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="S7" s="13" t="s">
+      <c r="S7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="T7" s="13" t="s">
+      <c r="T7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="U7" s="13" t="s">
+      <c r="U7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="V7" s="13" t="s">
+      <c r="V7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="W7" s="13" t="s">
+      <c r="W7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="X7" s="13" t="s">
+      <c r="X7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="Y7" s="13" t="s">
+      <c r="Y7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="Z7" s="13" t="s">
+      <c r="Z7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="AA7" s="13" t="s">
+      <c r="AA7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AB7" s="13" t="s">
+      <c r="AB7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AC7" s="13" t="s">
+      <c r="AC7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AD7" s="13" t="s">
+      <c r="AD7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AE7" s="13" t="s">
+      <c r="AE7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AF7" s="13" t="s">
+      <c r="AF7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="AG7" s="13" t="s">
+      <c r="AG7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AH7" s="15" t="s">
+      <c r="AH7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="AI7" s="14" t="s">
+      <c r="AI7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AJ7" s="14" t="s">
+      <c r="AJ7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AK7" s="14" t="s">
+      <c r="AK7" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:37" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
-      <c r="U8" s="9"/>
-      <c r="V8" s="9"/>
-      <c r="W8" s="9"/>
-      <c r="X8" s="9"/>
-      <c r="Y8" s="9"/>
-      <c r="Z8" s="9"/>
-      <c r="AA8" s="9"/>
-      <c r="AB8" s="9"/>
-      <c r="AC8" s="9"/>
-      <c r="AD8" s="9"/>
-      <c r="AE8" s="9"/>
-      <c r="AF8" s="9"/>
-      <c r="AG8" s="9"/>
-      <c r="AH8" s="11"/>
-      <c r="AI8" s="11"/>
-      <c r="AJ8" s="11"/>
-      <c r="AK8" s="11"/>
-    </row>
-    <row r="9" spans="1:37" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="7"/>
-      <c r="Z9" s="3"/>
-    </row>
-    <row r="10" spans="1:37" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="7"/>
-      <c r="Z10" s="3"/>
-    </row>
-    <row r="11" spans="1:37" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="7"/>
-      <c r="Z11" s="3"/>
+    <row r="8" spans="1:44" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="18"/>
+      <c r="T8" s="18"/>
+      <c r="U8" s="18"/>
+      <c r="V8" s="18"/>
+      <c r="W8" s="18"/>
+      <c r="X8" s="18"/>
+      <c r="Y8" s="18"/>
+      <c r="Z8" s="18"/>
+      <c r="AA8" s="18"/>
+      <c r="AB8" s="18"/>
+      <c r="AC8" s="18"/>
+      <c r="AD8" s="18"/>
+      <c r="AE8" s="18"/>
+      <c r="AF8" s="18"/>
+      <c r="AG8" s="18"/>
+      <c r="AH8" s="20"/>
+      <c r="AI8" s="20"/>
+      <c r="AJ8" s="20"/>
+      <c r="AK8" s="20"/>
+      <c r="AL8" s="15"/>
+      <c r="AM8" s="15"/>
+      <c r="AN8" s="15"/>
+      <c r="AO8" s="15"/>
+      <c r="AP8" s="15"/>
+      <c r="AQ8" s="15"/>
+      <c r="AR8" s="15"/>
+    </row>
+    <row r="9" spans="1:44" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
+      <c r="AA9" s="15"/>
+      <c r="AB9" s="15"/>
+      <c r="AC9" s="15"/>
+      <c r="AD9" s="15"/>
+      <c r="AE9" s="15"/>
+      <c r="AF9" s="15"/>
+      <c r="AG9" s="15"/>
+      <c r="AH9" s="15"/>
+      <c r="AI9" s="15"/>
+      <c r="AJ9" s="15"/>
+      <c r="AK9" s="15"/>
+      <c r="AL9" s="15"/>
+      <c r="AM9" s="15"/>
+      <c r="AN9" s="15"/>
+      <c r="AO9" s="15"/>
+      <c r="AP9" s="15"/>
+      <c r="AQ9" s="15"/>
+      <c r="AR9" s="15"/>
+    </row>
+    <row r="10" spans="1:44" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="15"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="15"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="15"/>
+      <c r="Y10" s="15"/>
+      <c r="Z10" s="15"/>
+      <c r="AA10" s="15"/>
+      <c r="AB10" s="15"/>
+      <c r="AC10" s="15"/>
+      <c r="AD10" s="15"/>
+      <c r="AE10" s="15"/>
+      <c r="AF10" s="15"/>
+      <c r="AG10" s="15"/>
+      <c r="AH10" s="15"/>
+      <c r="AI10" s="15"/>
+      <c r="AJ10" s="15"/>
+      <c r="AK10" s="15"/>
+      <c r="AL10" s="15"/>
+      <c r="AM10" s="15"/>
+      <c r="AN10" s="15"/>
+      <c r="AO10" s="15"/>
+      <c r="AP10" s="15"/>
+      <c r="AQ10" s="15"/>
+      <c r="AR10" s="15"/>
+    </row>
+    <row r="11" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="15"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
+      <c r="AA11" s="15"/>
+      <c r="AB11" s="15"/>
+      <c r="AC11" s="15"/>
+      <c r="AD11" s="15"/>
+      <c r="AE11" s="15"/>
+      <c r="AF11" s="15"/>
+      <c r="AG11" s="15"/>
+      <c r="AH11" s="15"/>
+      <c r="AI11" s="15"/>
+      <c r="AJ11" s="15"/>
+      <c r="AK11" s="15"/>
+      <c r="AL11" s="15"/>
+      <c r="AM11" s="15"/>
+      <c r="AN11" s="15"/>
+      <c r="AO11" s="15"/>
+      <c r="AP11" s="15"/>
+      <c r="AQ11" s="15"/>
+      <c r="AR11" s="15"/>
+    </row>
+    <row r="12" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
+      <c r="V12" s="15"/>
+      <c r="W12" s="15"/>
+      <c r="X12" s="15"/>
+      <c r="Y12" s="15"/>
+      <c r="Z12" s="15"/>
+      <c r="AA12" s="15"/>
+      <c r="AB12" s="15"/>
+      <c r="AC12" s="15"/>
+      <c r="AD12" s="15"/>
+      <c r="AE12" s="15"/>
+      <c r="AF12" s="15"/>
+      <c r="AG12" s="15"/>
+      <c r="AH12" s="15"/>
+      <c r="AI12" s="15"/>
+      <c r="AJ12" s="15"/>
+      <c r="AK12" s="15"/>
+      <c r="AL12" s="15"/>
+      <c r="AM12" s="15"/>
+      <c r="AN12" s="15"/>
+      <c r="AO12" s="15"/>
+      <c r="AP12" s="15"/>
+      <c r="AQ12" s="15"/>
+      <c r="AR12" s="15"/>
+    </row>
+    <row r="13" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="15"/>
+      <c r="Z13" s="15"/>
+      <c r="AA13" s="15"/>
+      <c r="AB13" s="15"/>
+      <c r="AC13" s="15"/>
+      <c r="AD13" s="15"/>
+      <c r="AE13" s="15"/>
+      <c r="AF13" s="15"/>
+      <c r="AG13" s="15"/>
+      <c r="AH13" s="15"/>
+      <c r="AI13" s="15"/>
+      <c r="AJ13" s="15"/>
+      <c r="AK13" s="15"/>
+      <c r="AL13" s="15"/>
+      <c r="AM13" s="15"/>
+      <c r="AN13" s="15"/>
+      <c r="AO13" s="15"/>
+      <c r="AP13" s="15"/>
+      <c r="AQ13" s="15"/>
+      <c r="AR13" s="15"/>
+    </row>
+    <row r="14" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
+      <c r="U14" s="15"/>
+      <c r="V14" s="15"/>
+      <c r="W14" s="15"/>
+      <c r="X14" s="15"/>
+      <c r="Y14" s="15"/>
+      <c r="Z14" s="15"/>
+      <c r="AA14" s="15"/>
+      <c r="AB14" s="15"/>
+      <c r="AC14" s="15"/>
+      <c r="AD14" s="15"/>
+      <c r="AE14" s="15"/>
+      <c r="AF14" s="15"/>
+      <c r="AG14" s="15"/>
+      <c r="AH14" s="15"/>
+      <c r="AI14" s="15"/>
+      <c r="AJ14" s="15"/>
+      <c r="AK14" s="15"/>
+      <c r="AL14" s="15"/>
+      <c r="AM14" s="15"/>
+      <c r="AN14" s="15"/>
+      <c r="AO14" s="15"/>
+      <c r="AP14" s="15"/>
+      <c r="AQ14" s="15"/>
+      <c r="AR14" s="15"/>
+    </row>
+    <row r="15" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="15"/>
+      <c r="U15" s="15"/>
+      <c r="V15" s="15"/>
+      <c r="W15" s="15"/>
+      <c r="X15" s="15"/>
+      <c r="Y15" s="15"/>
+      <c r="Z15" s="15"/>
+      <c r="AA15" s="15"/>
+      <c r="AB15" s="15"/>
+      <c r="AC15" s="15"/>
+      <c r="AD15" s="15"/>
+      <c r="AE15" s="15"/>
+      <c r="AF15" s="15"/>
+      <c r="AG15" s="15"/>
+      <c r="AH15" s="15"/>
+      <c r="AI15" s="15"/>
+      <c r="AJ15" s="15"/>
+      <c r="AK15" s="15"/>
+      <c r="AL15" s="15"/>
+      <c r="AM15" s="15"/>
+      <c r="AN15" s="15"/>
+      <c r="AO15" s="15"/>
+      <c r="AP15" s="15"/>
+      <c r="AQ15" s="15"/>
+      <c r="AR15" s="15"/>
+    </row>
+    <row r="16" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="15"/>
+      <c r="V16" s="15"/>
+      <c r="W16" s="15"/>
+      <c r="X16" s="15"/>
+      <c r="Y16" s="15"/>
+      <c r="Z16" s="15"/>
+      <c r="AA16" s="15"/>
+      <c r="AB16" s="15"/>
+      <c r="AC16" s="15"/>
+      <c r="AD16" s="15"/>
+      <c r="AE16" s="15"/>
+      <c r="AF16" s="15"/>
+      <c r="AG16" s="15"/>
+      <c r="AH16" s="15"/>
+      <c r="AI16" s="15"/>
+      <c r="AJ16" s="15"/>
+      <c r="AK16" s="15"/>
+      <c r="AL16" s="15"/>
+      <c r="AM16" s="15"/>
+      <c r="AN16" s="15"/>
+      <c r="AO16" s="15"/>
+      <c r="AP16" s="15"/>
+      <c r="AQ16" s="15"/>
+      <c r="AR16" s="15"/>
+    </row>
+    <row r="17" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="15"/>
+      <c r="U17" s="15"/>
+      <c r="V17" s="15"/>
+      <c r="W17" s="15"/>
+      <c r="X17" s="15"/>
+      <c r="Y17" s="15"/>
+      <c r="Z17" s="15"/>
+      <c r="AA17" s="15"/>
+      <c r="AB17" s="15"/>
+      <c r="AC17" s="15"/>
+      <c r="AD17" s="15"/>
+      <c r="AE17" s="15"/>
+      <c r="AF17" s="15"/>
+      <c r="AG17" s="15"/>
+      <c r="AH17" s="15"/>
+      <c r="AI17" s="15"/>
+      <c r="AJ17" s="15"/>
+      <c r="AK17" s="15"/>
+      <c r="AL17" s="15"/>
+      <c r="AM17" s="15"/>
+      <c r="AN17" s="15"/>
+      <c r="AO17" s="15"/>
+      <c r="AP17" s="15"/>
+      <c r="AQ17" s="15"/>
+      <c r="AR17" s="15"/>
+    </row>
+    <row r="18" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="15"/>
+      <c r="T18" s="15"/>
+      <c r="U18" s="15"/>
+      <c r="V18" s="15"/>
+      <c r="W18" s="15"/>
+      <c r="X18" s="15"/>
+      <c r="Y18" s="15"/>
+      <c r="Z18" s="15"/>
+      <c r="AA18" s="15"/>
+      <c r="AB18" s="15"/>
+      <c r="AC18" s="15"/>
+      <c r="AD18" s="15"/>
+      <c r="AE18" s="15"/>
+      <c r="AF18" s="15"/>
+      <c r="AG18" s="15"/>
+      <c r="AH18" s="15"/>
+      <c r="AI18" s="15"/>
+      <c r="AJ18" s="15"/>
+      <c r="AK18" s="15"/>
+      <c r="AL18" s="15"/>
+      <c r="AM18" s="15"/>
+      <c r="AN18" s="15"/>
+      <c r="AO18" s="15"/>
+      <c r="AP18" s="15"/>
+      <c r="AQ18" s="15"/>
+      <c r="AR18" s="15"/>
+    </row>
+    <row r="19" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
+      <c r="S19" s="15"/>
+      <c r="T19" s="15"/>
+      <c r="U19" s="15"/>
+      <c r="V19" s="15"/>
+      <c r="W19" s="15"/>
+      <c r="X19" s="15"/>
+      <c r="Y19" s="15"/>
+      <c r="Z19" s="15"/>
+      <c r="AA19" s="15"/>
+      <c r="AB19" s="15"/>
+      <c r="AC19" s="15"/>
+      <c r="AD19" s="15"/>
+      <c r="AE19" s="15"/>
+      <c r="AF19" s="15"/>
+      <c r="AG19" s="15"/>
+      <c r="AH19" s="15"/>
+      <c r="AI19" s="15"/>
+      <c r="AJ19" s="15"/>
+      <c r="AK19" s="15"/>
+      <c r="AL19" s="15"/>
+      <c r="AM19" s="15"/>
+      <c r="AN19" s="15"/>
+      <c r="AO19" s="15"/>
+      <c r="AP19" s="15"/>
+      <c r="AQ19" s="15"/>
+      <c r="AR19" s="15"/>
+    </row>
+    <row r="20" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15"/>
+      <c r="U20" s="15"/>
+      <c r="V20" s="15"/>
+      <c r="W20" s="15"/>
+      <c r="X20" s="15"/>
+      <c r="Y20" s="15"/>
+      <c r="Z20" s="15"/>
+      <c r="AA20" s="15"/>
+      <c r="AB20" s="15"/>
+      <c r="AC20" s="15"/>
+      <c r="AD20" s="15"/>
+      <c r="AE20" s="15"/>
+      <c r="AF20" s="15"/>
+      <c r="AG20" s="15"/>
+      <c r="AH20" s="15"/>
+      <c r="AI20" s="15"/>
+      <c r="AJ20" s="15"/>
+      <c r="AK20" s="15"/>
+      <c r="AL20" s="15"/>
+      <c r="AM20" s="15"/>
+      <c r="AN20" s="15"/>
+      <c r="AO20" s="15"/>
+      <c r="AP20" s="15"/>
+      <c r="AQ20" s="15"/>
+      <c r="AR20" s="15"/>
+    </row>
+    <row r="21" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="15"/>
+      <c r="T21" s="15"/>
+      <c r="U21" s="15"/>
+      <c r="V21" s="15"/>
+      <c r="W21" s="15"/>
+      <c r="X21" s="15"/>
+      <c r="Y21" s="15"/>
+      <c r="Z21" s="15"/>
+      <c r="AA21" s="15"/>
+      <c r="AB21" s="15"/>
+      <c r="AC21" s="15"/>
+      <c r="AD21" s="15"/>
+      <c r="AE21" s="15"/>
+      <c r="AF21" s="15"/>
+      <c r="AG21" s="15"/>
+      <c r="AH21" s="15"/>
+      <c r="AI21" s="15"/>
+      <c r="AJ21" s="15"/>
+      <c r="AK21" s="15"/>
+      <c r="AL21" s="15"/>
+      <c r="AM21" s="15"/>
+      <c r="AN21" s="15"/>
+      <c r="AO21" s="15"/>
+      <c r="AP21" s="15"/>
+      <c r="AQ21" s="15"/>
+      <c r="AR21" s="15"/>
+    </row>
+    <row r="22" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="15"/>
+      <c r="U22" s="15"/>
+      <c r="V22" s="15"/>
+      <c r="W22" s="15"/>
+      <c r="X22" s="15"/>
+      <c r="Y22" s="15"/>
+      <c r="Z22" s="15"/>
+      <c r="AA22" s="15"/>
+      <c r="AB22" s="15"/>
+      <c r="AC22" s="15"/>
+      <c r="AD22" s="15"/>
+      <c r="AE22" s="15"/>
+      <c r="AF22" s="15"/>
+      <c r="AG22" s="15"/>
+      <c r="AH22" s="15"/>
+      <c r="AI22" s="15"/>
+      <c r="AJ22" s="15"/>
+      <c r="AK22" s="15"/>
+      <c r="AL22" s="15"/>
+      <c r="AM22" s="15"/>
+      <c r="AN22" s="15"/>
+      <c r="AO22" s="15"/>
+      <c r="AP22" s="15"/>
+      <c r="AQ22" s="15"/>
+      <c r="AR22" s="15"/>
+    </row>
+    <row r="23" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="15"/>
+      <c r="T23" s="15"/>
+      <c r="U23" s="15"/>
+      <c r="V23" s="15"/>
+      <c r="W23" s="15"/>
+      <c r="X23" s="15"/>
+      <c r="Y23" s="15"/>
+      <c r="Z23" s="15"/>
+      <c r="AA23" s="15"/>
+      <c r="AB23" s="15"/>
+      <c r="AC23" s="15"/>
+      <c r="AD23" s="15"/>
+      <c r="AE23" s="15"/>
+      <c r="AF23" s="15"/>
+      <c r="AG23" s="15"/>
+      <c r="AH23" s="15"/>
+      <c r="AI23" s="15"/>
+      <c r="AJ23" s="15"/>
+      <c r="AK23" s="15"/>
+      <c r="AL23" s="15"/>
+      <c r="AM23" s="15"/>
+      <c r="AN23" s="15"/>
+      <c r="AO23" s="15"/>
+      <c r="AP23" s="15"/>
+      <c r="AQ23" s="15"/>
+      <c r="AR23" s="15"/>
+    </row>
+    <row r="24" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="17"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="15"/>
+      <c r="S24" s="15"/>
+      <c r="T24" s="15"/>
+      <c r="U24" s="15"/>
+      <c r="V24" s="15"/>
+      <c r="W24" s="15"/>
+      <c r="X24" s="15"/>
+      <c r="Y24" s="15"/>
+      <c r="Z24" s="15"/>
+      <c r="AA24" s="15"/>
+      <c r="AB24" s="15"/>
+      <c r="AC24" s="15"/>
+      <c r="AD24" s="15"/>
+      <c r="AE24" s="15"/>
+      <c r="AF24" s="15"/>
+      <c r="AG24" s="15"/>
+      <c r="AH24" s="15"/>
+      <c r="AI24" s="15"/>
+      <c r="AJ24" s="15"/>
+      <c r="AK24" s="15"/>
+      <c r="AL24" s="15"/>
+      <c r="AM24" s="15"/>
+      <c r="AN24" s="15"/>
+      <c r="AO24" s="15"/>
+      <c r="AP24" s="15"/>
+      <c r="AQ24" s="15"/>
+      <c r="AR24" s="15"/>
+    </row>
+    <row r="25" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="17"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="15"/>
+      <c r="S25" s="15"/>
+      <c r="T25" s="15"/>
+      <c r="U25" s="15"/>
+      <c r="V25" s="15"/>
+      <c r="W25" s="15"/>
+      <c r="X25" s="15"/>
+      <c r="Y25" s="15"/>
+      <c r="Z25" s="15"/>
+      <c r="AA25" s="15"/>
+      <c r="AB25" s="15"/>
+      <c r="AC25" s="15"/>
+      <c r="AD25" s="15"/>
+      <c r="AE25" s="15"/>
+      <c r="AF25" s="15"/>
+      <c r="AG25" s="15"/>
+      <c r="AH25" s="15"/>
+      <c r="AI25" s="15"/>
+      <c r="AJ25" s="15"/>
+      <c r="AK25" s="15"/>
+      <c r="AL25" s="15"/>
+      <c r="AM25" s="15"/>
+      <c r="AN25" s="15"/>
+      <c r="AO25" s="15"/>
+      <c r="AP25" s="15"/>
+      <c r="AQ25" s="15"/>
+      <c r="AR25" s="15"/>
+    </row>
+    <row r="26" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="17"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="15"/>
+      <c r="S26" s="15"/>
+      <c r="T26" s="15"/>
+      <c r="U26" s="15"/>
+      <c r="V26" s="15"/>
+      <c r="W26" s="15"/>
+      <c r="X26" s="15"/>
+      <c r="Y26" s="15"/>
+      <c r="Z26" s="15"/>
+      <c r="AA26" s="15"/>
+      <c r="AB26" s="15"/>
+      <c r="AC26" s="15"/>
+      <c r="AD26" s="15"/>
+      <c r="AE26" s="15"/>
+      <c r="AF26" s="15"/>
+      <c r="AG26" s="15"/>
+      <c r="AH26" s="15"/>
+      <c r="AI26" s="15"/>
+      <c r="AJ26" s="15"/>
+      <c r="AK26" s="15"/>
+      <c r="AL26" s="15"/>
+      <c r="AM26" s="15"/>
+      <c r="AN26" s="15"/>
+      <c r="AO26" s="15"/>
+      <c r="AP26" s="15"/>
+      <c r="AQ26" s="15"/>
+      <c r="AR26" s="15"/>
+    </row>
+    <row r="27" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="17"/>
+      <c r="O27" s="15"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="15"/>
+      <c r="R27" s="15"/>
+      <c r="S27" s="15"/>
+      <c r="T27" s="15"/>
+      <c r="U27" s="15"/>
+      <c r="V27" s="15"/>
+      <c r="W27" s="15"/>
+      <c r="X27" s="15"/>
+      <c r="Y27" s="15"/>
+      <c r="Z27" s="15"/>
+      <c r="AA27" s="15"/>
+      <c r="AB27" s="15"/>
+      <c r="AC27" s="15"/>
+      <c r="AD27" s="15"/>
+      <c r="AE27" s="15"/>
+      <c r="AF27" s="15"/>
+      <c r="AG27" s="15"/>
+      <c r="AH27" s="15"/>
+      <c r="AI27" s="15"/>
+      <c r="AJ27" s="15"/>
+      <c r="AK27" s="15"/>
+      <c r="AL27" s="15"/>
+      <c r="AM27" s="15"/>
+      <c r="AN27" s="15"/>
+      <c r="AO27" s="15"/>
+      <c r="AP27" s="15"/>
+      <c r="AQ27" s="15"/>
+      <c r="AR27" s="15"/>
+    </row>
+    <row r="28" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="17"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="15"/>
+      <c r="S28" s="15"/>
+      <c r="T28" s="15"/>
+      <c r="U28" s="15"/>
+      <c r="V28" s="15"/>
+      <c r="W28" s="15"/>
+      <c r="X28" s="15"/>
+      <c r="Y28" s="15"/>
+      <c r="Z28" s="15"/>
+      <c r="AA28" s="15"/>
+      <c r="AB28" s="15"/>
+      <c r="AC28" s="15"/>
+      <c r="AD28" s="15"/>
+      <c r="AE28" s="15"/>
+      <c r="AF28" s="15"/>
+      <c r="AG28" s="15"/>
+      <c r="AH28" s="15"/>
+      <c r="AI28" s="15"/>
+      <c r="AJ28" s="15"/>
+      <c r="AK28" s="15"/>
+      <c r="AL28" s="15"/>
+      <c r="AM28" s="15"/>
+      <c r="AN28" s="15"/>
+      <c r="AO28" s="15"/>
+      <c r="AP28" s="15"/>
+      <c r="AQ28" s="15"/>
+      <c r="AR28" s="15"/>
+    </row>
+    <row r="29" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="15"/>
+      <c r="R29" s="15"/>
+      <c r="S29" s="15"/>
+      <c r="T29" s="15"/>
+      <c r="U29" s="15"/>
+      <c r="V29" s="15"/>
+      <c r="W29" s="15"/>
+      <c r="X29" s="15"/>
+      <c r="Y29" s="15"/>
+      <c r="Z29" s="15"/>
+      <c r="AA29" s="15"/>
+      <c r="AB29" s="15"/>
+      <c r="AC29" s="15"/>
+      <c r="AD29" s="15"/>
+      <c r="AE29" s="15"/>
+      <c r="AF29" s="15"/>
+      <c r="AG29" s="15"/>
+      <c r="AH29" s="15"/>
+      <c r="AI29" s="15"/>
+      <c r="AJ29" s="15"/>
+      <c r="AK29" s="15"/>
+      <c r="AL29" s="15"/>
+      <c r="AM29" s="15"/>
+      <c r="AN29" s="15"/>
+      <c r="AO29" s="15"/>
+      <c r="AP29" s="15"/>
+      <c r="AQ29" s="15"/>
+      <c r="AR29" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
chia gang va export pdf
</commit_message>
<xml_diff>
--- a/Data_Product/App_Data/QTGN_Gang_Long_PKH.xlsx
+++ b/Data_Product/App_Data/QTGN_Gang_Long_PKH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_Projects\DATAPRODUCT\DATAPRODUCT\Data_Product\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60ED0BCC-0F0C-4BA4-B528-054CFB7E3771}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40570898-CEFA-4BBD-9E69-2C4E58CA2AA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12105" xr2:uid="{51577134-7CEF-4490-9A02-725D1462A1F6}"/>
   </bookViews>
@@ -310,15 +310,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -342,6 +333,15 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -704,7 +704,7 @@
   <dimension ref="A1:AS29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,104 +746,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:45" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="4" spans="1:45" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="11"/>
-      <c r="W4" s="11"/>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="11"/>
-      <c r="Z4" s="11"/>
-      <c r="AA4" s="11"/>
-      <c r="AB4" s="11"/>
-      <c r="AC4" s="11"/>
-      <c r="AD4" s="11"/>
-      <c r="AE4" s="11"/>
-      <c r="AF4" s="11"/>
-      <c r="AG4" s="11"/>
-      <c r="AH4" s="11"/>
-      <c r="AI4" s="11"/>
-      <c r="AJ4" s="11"/>
-      <c r="AK4" s="11"/>
-      <c r="AL4" s="11"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="19"/>
+      <c r="W4" s="19"/>
+      <c r="X4" s="19"/>
+      <c r="Y4" s="19"/>
+      <c r="Z4" s="19"/>
+      <c r="AA4" s="19"/>
+      <c r="AB4" s="19"/>
+      <c r="AC4" s="19"/>
+      <c r="AD4" s="19"/>
+      <c r="AE4" s="19"/>
+      <c r="AF4" s="19"/>
+      <c r="AG4" s="19"/>
+      <c r="AH4" s="19"/>
+      <c r="AI4" s="19"/>
+      <c r="AJ4" s="19"/>
+      <c r="AK4" s="19"/>
+      <c r="AL4" s="19"/>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="9"/>
-      <c r="W5" s="9"/>
-      <c r="X5" s="9"/>
-      <c r="Y5" s="9"/>
-      <c r="Z5" s="9"/>
-      <c r="AA5" s="9"/>
-      <c r="AB5" s="9"/>
-      <c r="AC5" s="9"/>
-      <c r="AD5" s="9"/>
-      <c r="AE5" s="9"/>
-      <c r="AF5" s="9"/>
-      <c r="AG5" s="9"/>
-      <c r="AH5" s="9"/>
-      <c r="AI5" s="9"/>
-      <c r="AJ5" s="9"/>
-      <c r="AK5" s="9"/>
-      <c r="AL5" s="9"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
+      <c r="U5" s="17"/>
+      <c r="V5" s="17"/>
+      <c r="W5" s="17"/>
+      <c r="X5" s="17"/>
+      <c r="Y5" s="17"/>
+      <c r="Z5" s="17"/>
+      <c r="AA5" s="17"/>
+      <c r="AB5" s="17"/>
+      <c r="AC5" s="17"/>
+      <c r="AD5" s="17"/>
+      <c r="AE5" s="17"/>
+      <c r="AF5" s="17"/>
+      <c r="AG5" s="17"/>
+      <c r="AH5" s="17"/>
+      <c r="AI5" s="17"/>
+      <c r="AJ5" s="17"/>
+      <c r="AK5" s="17"/>
+      <c r="AL5" s="17"/>
     </row>
     <row r="7" spans="1:45" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -894,112 +894,112 @@
       <c r="P7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="Q7" s="12" t="s">
+      <c r="Q7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="R7" s="12" t="s">
+      <c r="R7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="S7" s="13" t="s">
+      <c r="S7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="T7" s="13" t="s">
+      <c r="T7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="U7" s="13" t="s">
+      <c r="U7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="V7" s="13" t="s">
+      <c r="V7" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="W7" s="13" t="s">
+      <c r="W7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="X7" s="13" t="s">
+      <c r="X7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="Y7" s="13" t="s">
+      <c r="Y7" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="Z7" s="13" t="s">
+      <c r="Z7" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AA7" s="13" t="s">
+      <c r="AA7" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="AB7" s="13" t="s">
+      <c r="AB7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="AC7" s="13" t="s">
+      <c r="AC7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="AD7" s="13" t="s">
+      <c r="AD7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="AE7" s="13" t="s">
+      <c r="AE7" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="AF7" s="13" t="s">
+      <c r="AF7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="AG7" s="13" t="s">
+      <c r="AG7" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="AH7" s="13" t="s">
+      <c r="AH7" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="AI7" s="14" t="s">
+      <c r="AI7" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AJ7" s="15" t="s">
+      <c r="AJ7" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="AK7" s="15" t="s">
+      <c r="AK7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="AL7" s="15" t="s">
+      <c r="AL7" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:45" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="16"/>
-      <c r="T8" s="16"/>
-      <c r="U8" s="16"/>
-      <c r="V8" s="16"/>
-      <c r="W8" s="16"/>
-      <c r="X8" s="16"/>
-      <c r="Y8" s="16"/>
-      <c r="Z8" s="16"/>
-      <c r="AA8" s="16"/>
-      <c r="AB8" s="16"/>
-      <c r="AC8" s="16"/>
-      <c r="AD8" s="16"/>
-      <c r="AE8" s="16"/>
-      <c r="AF8" s="16"/>
-      <c r="AG8" s="16"/>
-      <c r="AH8" s="16"/>
-      <c r="AI8" s="18"/>
-      <c r="AJ8" s="18"/>
-      <c r="AK8" s="18"/>
-      <c r="AL8" s="18"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="13"/>
+      <c r="X8" s="13"/>
+      <c r="Y8" s="13"/>
+      <c r="Z8" s="13"/>
+      <c r="AA8" s="13"/>
+      <c r="AB8" s="13"/>
+      <c r="AC8" s="13"/>
+      <c r="AD8" s="13"/>
+      <c r="AE8" s="13"/>
+      <c r="AF8" s="13"/>
+      <c r="AG8" s="13"/>
+      <c r="AH8" s="13"/>
+      <c r="AI8" s="15"/>
+      <c r="AJ8" s="15"/>
+      <c r="AK8" s="15"/>
+      <c r="AL8" s="15"/>
       <c r="AM8" s="5"/>
       <c r="AN8" s="5"/>
       <c r="AO8" s="5"/>

</xml_diff>